<commit_message>
Changed Excel data to remove type error for manager_id field
</commit_message>
<xml_diff>
--- a/IntranetApplication/associates.xlsx
+++ b/IntranetApplication/associates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDK_InternalApps\IntranetApplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntranetApp\IntranetApplication\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>kumarar</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Manish.Singh@cdk.com</t>
-  </si>
-  <si>
-    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -402,9 +399,6 @@
       <c r="E1" t="b">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>

<commit_message>
Added records in excel
</commit_message>
<xml_diff>
--- a/IntranetApplication/associates.xlsx
+++ b/IntranetApplication/associates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>kumarar</t>
   </si>
@@ -42,6 +42,24 @@
   </si>
   <si>
     <t>Manish.Singh@cdk.com</t>
+  </si>
+  <si>
+    <t>pullurul</t>
+  </si>
+  <si>
+    <t>Likhitha Pulluru</t>
+  </si>
+  <si>
+    <t>Likhitha.Pulluru@cdk.com</t>
+  </si>
+  <si>
+    <t>Sowmya Golla</t>
+  </si>
+  <si>
+    <t>Sowmya.Golla@cdk.com</t>
+  </si>
+  <si>
+    <t>gollas</t>
   </si>
 </sst>
 </file>
@@ -370,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +403,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>201234</v>
+        <v>403121</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -417,14 +435,57 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>201234</v>
+        <v>403121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>501302</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>403121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>501278</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>403121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D1" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replaced sql cmds with django queryset api cmds and UI cleanup
</commit_message>
<xml_diff>
--- a/IntranetApplication/associates.xlsx
+++ b/IntranetApplication/associates.xlsx
@@ -41,25 +41,25 @@
     <t>Manish Singh</t>
   </si>
   <si>
+    <t>pullurul</t>
+  </si>
+  <si>
+    <t>Likhitha Pulluru</t>
+  </si>
+  <si>
+    <t>Sowmya Golla</t>
+  </si>
+  <si>
+    <t>Sowmya.Golla@cdk.com</t>
+  </si>
+  <si>
+    <t>gollas</t>
+  </si>
+  <si>
+    <t>Likitha.pulluru@cdk.com</t>
+  </si>
+  <si>
     <t>Manish.Singh@cdk.com</t>
-  </si>
-  <si>
-    <t>pullurul</t>
-  </si>
-  <si>
-    <t>Likhitha Pulluru</t>
-  </si>
-  <si>
-    <t>Likhitha.Pulluru@cdk.com</t>
-  </si>
-  <si>
-    <t>Sowmya Golla</t>
-  </si>
-  <si>
-    <t>Sowmya.Golla@cdk.com</t>
-  </si>
-  <si>
-    <t>gollas</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E1" t="b">
         <v>1</v>
@@ -443,13 +443,13 @@
         <v>501302</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -463,13 +463,13 @@
         <v>501278</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -481,9 +481,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D1" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId2"/>
     <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D1" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>